<commit_message>
SE ANEXA ACTUALIZACION DEL FORMATO OBJETIVOS-ARTEFACTOS DE ANALISIS Y CARPETA SPRINT 2 CON FORMATO DE SEGUIMIENTO
</commit_message>
<xml_diff>
--- a/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
+++ b/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/SPRINT1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EE9666-8DE9-7140-BF80-9D0026AD93B6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAD4A38-E75B-DB4E-9664-F6B2B141C413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME SPRINT" sheetId="12" r:id="rId1"/>
-    <sheet name="REUNION 27-08-2022" sheetId="15" r:id="rId2"/>
-    <sheet name="REUNION 25-08-2022" sheetId="14" r:id="rId3"/>
-    <sheet name="REUNION 24-08-2022" sheetId="13" r:id="rId4"/>
-    <sheet name="REUNION 23-08-2022" sheetId="11" r:id="rId5"/>
-    <sheet name="DISTRIBUCION 21-08-2022" sheetId="10" r:id="rId6"/>
-    <sheet name="PLANEACION 21-08-2022" sheetId="9" r:id="rId7"/>
+    <sheet name="REUNION 28-08-2022" sheetId="16" r:id="rId2"/>
+    <sheet name="REUNION 27-08-2022" sheetId="15" r:id="rId3"/>
+    <sheet name="REUNION 25-08-2022" sheetId="14" r:id="rId4"/>
+    <sheet name="REUNION 24-08-2022" sheetId="13" r:id="rId5"/>
+    <sheet name="REUNION 23-08-2022" sheetId="11" r:id="rId6"/>
+    <sheet name="DISTRIBUCION 21-08-2022" sheetId="10" r:id="rId7"/>
+    <sheet name="PLANEACION 21-08-2022" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="54">
   <si>
     <t>HACER</t>
   </si>
@@ -196,9 +198,6 @@
     <t>Miembro del equipo anuncia su retiro del programa</t>
   </si>
   <si>
-    <t>Se distribuye la actividad asignada de ese miembro entre todos los miembros</t>
-  </si>
-  <si>
     <t>Excel</t>
   </si>
   <si>
@@ -206,6 +205,9 @@
   </si>
   <si>
     <t>OBJETIVOS METOLOGIA - SOFTWARE Y FORMATOS - ARTEFACTOS ANALISIS</t>
+  </si>
+  <si>
+    <t>Se distribuye la actividad asignada de ese miembro entre todos los miembros del equipo</t>
   </si>
 </sst>
 </file>
@@ -213,7 +215,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -608,7 +610,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +650,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -666,26 +678,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -696,53 +726,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="102">
+  <dxfs count="119">
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -814,6 +861,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -884,6 +961,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -954,6 +1061,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1024,6 +1161,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1094,6 +1261,36 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -1167,181 +1364,89 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1357,15 +1462,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Tabla134756" displayName="Tabla134756" ref="A1:F8" totalsRowCount="1" headerRowDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DAF9B008-E008-A544-84D7-8559DC8E169A}" name="Tabla1347568" displayName="Tabla1347568" ref="A1:F8" totalsRowCount="1" headerRowDxfId="111">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{43B31EA2-5033-124E-8730-3071676C1780}" name="ID" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{0F148B97-27DE-FB48-8679-E90DD74E6947}" name="VALOR" totalsRowDxfId="45" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{2E315A6F-7724-3D46-84AA-335A70295795}" name="ACTIVIDAD" dataDxfId="49" totalsRowDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{18F811EF-CDDD-DB4A-AA38-F633528B3EA2}" name="RESPONSABLE" dataDxfId="48" totalsRowDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{12BAB512-F0DF-AE43-AB16-88A2C41D1157}" name="ESTADO" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{A3485E03-CCF8-134C-B5A2-953813DDFB7B}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="46" totalsRowDxfId="42" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{5C096F99-9B91-DE40-878E-814BDFEB9846}" name="ID" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{0F0E58AE-6A00-FC45-AE94-EA6D436976B9}" name="VALOR" totalsRowDxfId="3" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{18DA65E6-568E-6C4F-ACA7-45CAACFA2F57}" name="ACTIVIDAD" dataDxfId="109" totalsRowDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D5B7DF44-BD95-454D-B6F6-6601063DE794}" name="RESPONSABLE" dataDxfId="108" totalsRowDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{3FAAD558-904B-DD40-920C-627F98A8C8D5}" name="ESTADO" dataDxfId="107"/>
+    <tableColumn id="4" xr3:uid="{ED810AD6-1A4E-FF44-ADA4-0F9B58BF457A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+      <calculatedColumnFormula>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Tabla134756" displayName="Tabla134756" ref="A1:F8" totalsRowCount="1" headerRowDxfId="98">
+  <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{43B31EA2-5033-124E-8730-3071676C1780}" name="ID" dataDxfId="97"/>
+    <tableColumn id="5" xr3:uid="{0F148B97-27DE-FB48-8679-E90DD74E6947}" name="VALOR" totalsRowDxfId="96" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{2E315A6F-7724-3D46-84AA-335A70295795}" name="ACTIVIDAD" dataDxfId="95" totalsRowDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{18F811EF-CDDD-DB4A-AA38-F633528B3EA2}" name="RESPONSABLE" dataDxfId="93" totalsRowDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{12BAB512-F0DF-AE43-AB16-88A2C41D1157}" name="ESTADO" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{A3485E03-CCF8-134C-B5A2-953813DDFB7B}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1373,16 +1495,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Tabla13475" displayName="Tabla13475" ref="A1:F8" totalsRowCount="1" headerRowDxfId="101">
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Tabla13475" displayName="Tabla13475" ref="A1:F8" totalsRowCount="1" headerRowDxfId="81">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B4847248-0602-FF41-ADA7-0593C164551A}" name="ID" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{9570677A-6887-D04B-BC98-FDBF6E642A8E}" name="VALOR" totalsRowDxfId="99" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{F2ACB2B9-3C20-3C4C-86F6-9F569FFCD182}" name="ACTIVIDAD" dataDxfId="98" totalsRowDxfId="97"/>
-    <tableColumn id="6" xr3:uid="{92E380FF-D61D-F04A-83C3-F3A28156C5B7}" name="RESPONSABLE" dataDxfId="96" totalsRowDxfId="95"/>
-    <tableColumn id="3" xr3:uid="{D38B5B8B-4C15-1F44-9B50-D2E36B73D937}" name="ESTADO" dataDxfId="94"/>
-    <tableColumn id="4" xr3:uid="{4229043C-4974-C04E-BCD3-F4185B2BE02C}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="93" totalsRowDxfId="92" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{B4847248-0602-FF41-ADA7-0593C164551A}" name="ID" dataDxfId="80"/>
+    <tableColumn id="5" xr3:uid="{9570677A-6887-D04B-BC98-FDBF6E642A8E}" name="VALOR" totalsRowDxfId="79" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{F2ACB2B9-3C20-3C4C-86F6-9F569FFCD182}" name="ACTIVIDAD" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="6" xr3:uid="{92E380FF-D61D-F04A-83C3-F3A28156C5B7}" name="RESPONSABLE" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{D38B5B8B-4C15-1F44-9B50-D2E36B73D937}" name="ESTADO" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{4229043C-4974-C04E-BCD3-F4185B2BE02C}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1390,16 +1512,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Tabla1347" displayName="Tabla1347" ref="A1:F8" totalsRowCount="1" headerRowDxfId="91">
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Tabla1347" displayName="Tabla1347" ref="A1:F8" totalsRowCount="1" headerRowDxfId="64">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8530F876-5333-8C42-9B99-E7524B03868D}" name="ID" dataDxfId="90"/>
-    <tableColumn id="5" xr3:uid="{0B425CEF-57FA-0449-9D48-799937F316DA}" name="VALOR" totalsRowDxfId="89" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{A86CCCCE-9767-BA45-8D59-EA4E2B8A125F}" name="ACTIVIDAD" dataDxfId="88" totalsRowDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{2D321822-E2C3-774D-8799-C0A2CC73F8D9}" name="RESPONSABLE" dataDxfId="86" totalsRowDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{6FFC2B3E-2017-BA44-8965-136231A0E04B}" name="ESTADO" dataDxfId="84"/>
-    <tableColumn id="4" xr3:uid="{A4DFDF0B-96A1-C44C-9DCA-957651D5921A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="83" totalsRowDxfId="82" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{8530F876-5333-8C42-9B99-E7524B03868D}" name="ID" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{0B425CEF-57FA-0449-9D48-799937F316DA}" name="VALOR" totalsRowDxfId="62" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{A86CCCCE-9767-BA45-8D59-EA4E2B8A125F}" name="ACTIVIDAD" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{2D321822-E2C3-774D-8799-C0A2CC73F8D9}" name="RESPONSABLE" dataDxfId="59" totalsRowDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{6FFC2B3E-2017-BA44-8965-136231A0E04B}" name="ESTADO" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{A4DFDF0B-96A1-C44C-9DCA-957651D5921A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1407,16 +1529,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Tabla134" displayName="Tabla134" ref="A1:F8" totalsRowCount="1" headerRowDxfId="81">
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Tabla134" displayName="Tabla134" ref="A1:F8" totalsRowCount="1" headerRowDxfId="47">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1F035DC9-1373-3E4C-A3A8-13DBEC76DC82}" name="ID" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{43A5529E-007E-C64C-86CE-8DAB48DE5353}" name="VALOR" totalsRowDxfId="79" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{9A1D5E6B-0F9C-014B-BC79-0CE8E35ABDF2}" name="ACTIVIDAD" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{9DE32ABE-C5F1-6641-97D6-E5E2D7B798CA}" name="RESPONSABLE" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{669DC672-6610-F249-B210-DEC4DB36456B}" name="ESTADO" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{2EC93C66-3A32-2A40-B7A6-F121B89B9430}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{1F035DC9-1373-3E4C-A3A8-13DBEC76DC82}" name="ID" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{43A5529E-007E-C64C-86CE-8DAB48DE5353}" name="VALOR" totalsRowDxfId="45" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{9A1D5E6B-0F9C-014B-BC79-0CE8E35ABDF2}" name="ACTIVIDAD" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{9DE32ABE-C5F1-6641-97D6-E5E2D7B798CA}" name="RESPONSABLE" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{669DC672-6610-F249-B210-DEC4DB36456B}" name="ESTADO" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{2EC93C66-3A32-2A40-B7A6-F121B89B9430}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1424,16 +1546,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Tabla13" displayName="Tabla13" ref="A1:F8" totalsRowCount="1" headerRowDxfId="71">
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Tabla13" displayName="Tabla13" ref="A1:F8" totalsRowCount="1" headerRowDxfId="30">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C6E86F07-4CB4-4546-AD18-8C75028994F5}" name="ID" dataDxfId="70"/>
-    <tableColumn id="5" xr3:uid="{DBCD9DEA-ACBA-874C-A22B-59D086F3B877}" name="VALOR" totalsRowDxfId="69" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{D1E5958A-BF8A-BF45-BC61-F88DD4F0DC31}" name="ACTIVIDAD" dataDxfId="68" totalsRowDxfId="67"/>
-    <tableColumn id="6" xr3:uid="{300B975F-DA35-4641-AFFB-C25636AED70A}" name="RESPONSABLE" dataDxfId="66" totalsRowDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{55C19C11-970E-ED48-9E1D-FD413A44DB58}" name="ESTADO" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{F26AE47E-E038-0B42-868B-70E1B4FF0502}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{C6E86F07-4CB4-4546-AD18-8C75028994F5}" name="ID" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{DBCD9DEA-ACBA-874C-A22B-59D086F3B877}" name="VALOR" totalsRowDxfId="28" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{D1E5958A-BF8A-BF45-BC61-F88DD4F0DC31}" name="ACTIVIDAD" dataDxfId="27" totalsRowDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{300B975F-DA35-4641-AFFB-C25636AED70A}" name="RESPONSABLE" dataDxfId="25" totalsRowDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{55C19C11-970E-ED48-9E1D-FD413A44DB58}" name="ESTADO" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{F26AE47E-E038-0B42-868B-70E1B4FF0502}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1441,16 +1563,16 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="61">
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="13">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B00B770C-E8F2-CB46-A39B-1F22E5737A8F}" name="ID" dataDxfId="60"/>
-    <tableColumn id="5" xr3:uid="{5618240B-7421-2E49-B85A-37682FDA546C}" name="VALOR" totalsRowDxfId="59" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{FD0BACDA-4B7C-AE4A-B6CC-54F3CF36C08D}" name="ACTIVIDAD" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{FD255310-A28E-5448-BD5D-4F7B55D7AFCB}" name="RESPONSABLE" dataDxfId="56" totalsRowDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{EDB2A1F3-0893-E44D-BCDD-5AACC2B519F8}" name="ESTADO" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{684EEF9A-6840-2141-90A0-69B802ECABA8}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="53" totalsRowDxfId="52" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{B00B770C-E8F2-CB46-A39B-1F22E5737A8F}" name="ID" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{5618240B-7421-2E49-B85A-37682FDA546C}" name="VALOR" totalsRowDxfId="11" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{FD0BACDA-4B7C-AE4A-B6CC-54F3CF36C08D}" name="ACTIVIDAD" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{FD255310-A28E-5448-BD5D-4F7B55D7AFCB}" name="RESPONSABLE" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{EDB2A1F3-0893-E44D-BCDD-5AACC2B519F8}" name="ESTADO" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{684EEF9A-6840-2141-90A0-69B802ECABA8}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1724,7 +1846,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="G11" sqref="G11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1750,230 +1872,230 @@
       <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="29"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="27" t="s">
+      <c r="G1" s="49"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="19">
+      <c r="A2" s="23">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="26"/>
+      <c r="F2" s="42" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="43"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="F2" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="27"/>
+      <c r="F3" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="43"/>
+      <c r="H3" s="44"/>
+      <c r="I3" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="20"/>
-      <c r="B3" s="42"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="23"/>
-      <c r="F3" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="33"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="20"/>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="23"/>
-      <c r="F4" s="32" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="27"/>
+      <c r="F4" s="42" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="33"/>
-      <c r="H4" s="34"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="44"/>
       <c r="I4" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="20"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="23"/>
-      <c r="F5" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="33"/>
-      <c r="H5" s="34"/>
+      <c r="A5" s="24"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="27"/>
+      <c r="F5" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="43"/>
+      <c r="H5" s="44"/>
       <c r="I5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="23"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="34"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="27"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
       <c r="I6" s="2"/>
     </row>
     <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="24"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="25">
+      <c r="A8" s="35">
         <v>2</v>
       </c>
-      <c r="B8" s="45"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="26"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="36"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="46"/>
-      <c r="C9" s="46"/>
-      <c r="D9" s="23"/>
-      <c r="F9" s="35" t="s">
+      <c r="A9" s="24"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="27"/>
+      <c r="F9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="31" t="s">
+      <c r="G9" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
-      <c r="B10" s="47"/>
-      <c r="C10" s="47"/>
-      <c r="D10" s="23"/>
-      <c r="F10" s="35" t="s">
+      <c r="A10" s="24"/>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39"/>
+      <c r="D10" s="27"/>
+      <c r="F10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="46">
         <v>44798</v>
       </c>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="46"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="23"/>
-      <c r="F11" s="35" t="s">
+      <c r="A11" s="24"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="27"/>
+      <c r="F11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="H11" s="47"/>
+      <c r="I11" s="47"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47"/>
-      <c r="D12" s="23"/>
+      <c r="A12" s="24"/>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="27"/>
     </row>
     <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="24"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="41"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="28"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="19">
+      <c r="A14" s="23">
         <v>3</v>
       </c>
-      <c r="B14" s="49"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="22"/>
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
-      <c r="B15" s="46"/>
-      <c r="C15" s="46"/>
-      <c r="D15" s="23"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
-      <c r="B16" s="47"/>
-      <c r="C16" s="47"/>
-      <c r="D16" s="23"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="39"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="27"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="20"/>
-      <c r="B17" s="46"/>
-      <c r="C17" s="46"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="27"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
-      <c r="B18" s="47"/>
-      <c r="C18" s="47"/>
-      <c r="D18" s="23"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39"/>
+      <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21"/>
-      <c r="B19" s="48"/>
-      <c r="C19" s="48"/>
-      <c r="D19" s="24"/>
+      <c r="A19" s="25"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="28"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="19">
+      <c r="A20" s="23">
         <v>4</v>
       </c>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="22"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="46"/>
-      <c r="C21" s="46"/>
-      <c r="D21" s="23"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
-      <c r="B22" s="47"/>
-      <c r="C22" s="47"/>
-      <c r="D22" s="23"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="39"/>
+      <c r="C22" s="39"/>
+      <c r="D22" s="27"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="20"/>
-      <c r="B23" s="46"/>
-      <c r="C23" s="46"/>
-      <c r="D23" s="23"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="38"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="27"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
-      <c r="B24" s="47"/>
-      <c r="C24" s="47"/>
-      <c r="D24" s="23"/>
+      <c r="A24" s="24"/>
+      <c r="B24" s="39"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="27"/>
     </row>
     <row r="25" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21"/>
-      <c r="B25" s="48"/>
-      <c r="C25" s="48"/>
-      <c r="D25" s="24"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="41"/>
+      <c r="D25" s="28"/>
       <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2029,10 +2151,315 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F45049-B0C9-8441-BE8F-F70E663206EB}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="str">
+        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="7">
+        <f>SUBTOTAL(109,Tabla1347568[PROGRESO])</f>
+        <v>0.85000000000000009</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <f>COUNTIF(Tabla1347568[ESTADO],"HACER")</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <f>COUNTIF(Tabla1347568[ESTADO],"HACIENDO")</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="22">
+        <v>1</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <f>COUNTIF(Tabla1347568[ESTADO],"VERIFICAR")</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="22">
+        <v>2</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3">
+        <f>COUNTIF(Tabla1347568[ESTADO],"HECHO")</f>
+        <v>5</v>
+      </c>
+      <c r="F14" s="22">
+        <v>3</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F15" s="22">
+        <v>4</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="5" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="6" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="7" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="2" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{173F3A64-8499-FE46-8D27-CA94C26E5A89}">
+      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{72532A5C-9CE8-FE40-826C-5A123CFDB9D6}">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A8DC1C-B48E-3D45-8831-0A62DF6933FD}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
@@ -2228,13 +2655,13 @@
         <f>COUNTIF(Tabla134756[ESTADO],"HACIENDO")</f>
         <v>2</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2246,7 +2673,7 @@
         <f>COUNTIF(Tabla134756[ESTADO],"VERIFICAR")</f>
         <v>1</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -2264,7 +2691,7 @@
         <f>COUNTIF(Tabla134756[ESTADO],"HECHO")</f>
         <v>3</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -2275,7 +2702,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -2293,28 +2720,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="41" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="105" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="104" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="102" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="37" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="100" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2333,7 +2760,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A12336-19D1-7A49-A729-A680FE050C77}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -2533,13 +2960,13 @@
         <f>COUNTIF(Tabla13475[ESTADO],"HACIENDO")</f>
         <v>1</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2551,7 +2978,7 @@
         <f>COUNTIF(Tabla13475[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -2569,7 +2996,7 @@
         <f>COUNTIF(Tabla13475[ESTADO],"HECHO")</f>
         <v>2</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -2580,7 +3007,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -2598,28 +3025,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="34" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="88" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="87" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="86" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="85" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="83" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2638,7 +3065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA48102-9501-E841-A6C2-864B0ECAAC64}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -2838,13 +3265,13 @@
         <f>COUNTIF(Tabla1347[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2856,7 +3283,7 @@
         <f>COUNTIF(Tabla1347[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -2874,7 +3301,7 @@
         <f>COUNTIF(Tabla1347[ESTADO],"HECHO")</f>
         <v>1</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -2885,7 +3312,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -2903,28 +3330,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="27" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="71" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="70" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="68" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="23" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="66" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2943,7 +3370,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FEBE19-1B7C-E447-8CE1-7FE68E40E356}">
   <dimension ref="A1:H17"/>
   <sheetViews>
@@ -3143,13 +3570,13 @@
         <f>COUNTIF(Tabla134[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3161,7 +3588,7 @@
         <f>COUNTIF(Tabla134[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3179,7 +3606,7 @@
         <f>COUNTIF(Tabla134[ESTADO],"HECHO")</f>
         <v>1</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3190,7 +3617,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3208,28 +3635,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="20" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="52" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="51" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="49" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3248,7 +3675,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FDAD686-6E10-C14E-8CCB-E532B3077046}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -3447,13 +3874,13 @@
         <f>COUNTIF(Tabla13[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3465,7 +3892,7 @@
         <f>COUNTIF(Tabla13[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3483,7 +3910,7 @@
         <f>COUNTIF(Tabla13[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3494,7 +3921,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3506,28 +3933,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3546,7 +3973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1BC46D-31D7-9346-BF0C-A8183120C5EB}">
   <dimension ref="A1:H19"/>
   <sheetViews>
@@ -3723,13 +4150,13 @@
         <f>COUNTIF(Tabla1[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="38">
+      <c r="F12" s="22">
         <v>1</v>
       </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3741,7 +4168,7 @@
         <f>COUNTIF(Tabla1[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="38">
+      <c r="F13" s="22">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3759,7 +4186,7 @@
         <f>COUNTIF(Tabla1[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
-      <c r="F14" s="38">
+      <c r="F14" s="22">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3770,7 +4197,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="38">
+      <c r="F15" s="22">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3786,28 +4213,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="6" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="7" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="11" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="12" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SE ANEXA ACTUALIZACION DEL FORMATO DE SEGUIMIENTO SPRINT1 CON PROGRESO ACTUAL Y EVIDENCIAS
</commit_message>
<xml_diff>
--- a/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
+++ b/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/SPRINT1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EAD4A38-E75B-DB4E-9664-F6B2B141C413}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B80E128-2EEB-8B44-806C-30611974EE35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,6 @@
     <sheet name="PLANEACION 21-08-2022" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -660,6 +659,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -702,46 +741,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -752,15 +751,103 @@
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
@@ -773,15 +860,115 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -873,15 +1060,115 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -1083,294 +1370,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1461,16 +1460,265 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>159159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3006791</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAF2F694-4B2C-1445-99B9-5D81F97E314C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8712200" y="2851559"/>
+          <a:ext cx="2867091" cy="1771241"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>159159</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2955991</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0923D6E3-65F0-4C43-9323-AE51AEF5F48D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8661400" y="2851559"/>
+          <a:ext cx="2867091" cy="1771241"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>101599</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>136524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3053078</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagen 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6954F654-DDEA-4440-A6E2-D43914A55DED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8674099" y="5114924"/>
+          <a:ext cx="2951479" cy="1844675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>222248</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3020062</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>165099</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagen 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FEE6307-2764-014F-8121-748DC1D858E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8636000" y="7486648"/>
+          <a:ext cx="2956562" cy="1847851"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>48260</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>203200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>3035300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagen 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A9689E5-905D-2B4E-A814-AF6D73B77C70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8620760" y="609600"/>
+          <a:ext cx="2987040" cy="1866900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DAF9B008-E008-A544-84D7-8559DC8E169A}" name="Tabla1347568" displayName="Tabla1347568" ref="A1:F8" totalsRowCount="1" headerRowDxfId="111">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5C096F99-9B91-DE40-878E-814BDFEB9846}" name="ID" dataDxfId="110"/>
-    <tableColumn id="5" xr3:uid="{0F0E58AE-6A00-FC45-AE94-EA6D436976B9}" name="VALOR" totalsRowDxfId="3" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{18DA65E6-568E-6C4F-ACA7-45CAACFA2F57}" name="ACTIVIDAD" dataDxfId="109" totalsRowDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{D5B7DF44-BD95-454D-B6F6-6601063DE794}" name="RESPONSABLE" dataDxfId="108" totalsRowDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{3FAAD558-904B-DD40-920C-627F98A8C8D5}" name="ESTADO" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{ED810AD6-1A4E-FF44-ADA4-0F9B58BF457A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="106" totalsRowDxfId="0" dataCellStyle="Porcentaje">
+    <tableColumn id="5" xr3:uid="{0F0E58AE-6A00-FC45-AE94-EA6D436976B9}" name="VALOR" totalsRowDxfId="109" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{18DA65E6-568E-6C4F-ACA7-45CAACFA2F57}" name="ACTIVIDAD" dataDxfId="108" totalsRowDxfId="107"/>
+    <tableColumn id="6" xr3:uid="{D5B7DF44-BD95-454D-B6F6-6601063DE794}" name="RESPONSABLE" dataDxfId="106" totalsRowDxfId="105"/>
+    <tableColumn id="3" xr3:uid="{3FAAD558-904B-DD40-920C-627F98A8C8D5}" name="ESTADO" dataDxfId="104"/>
+    <tableColumn id="4" xr3:uid="{ED810AD6-1A4E-FF44-ADA4-0F9B58BF457A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1479,15 +1727,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Tabla134756" displayName="Tabla134756" ref="A1:F8" totalsRowCount="1" headerRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Tabla134756" displayName="Tabla134756" ref="A1:F8" totalsRowCount="1" headerRowDxfId="94">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{43B31EA2-5033-124E-8730-3071676C1780}" name="ID" dataDxfId="97"/>
-    <tableColumn id="5" xr3:uid="{0F148B97-27DE-FB48-8679-E90DD74E6947}" name="VALOR" totalsRowDxfId="96" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{2E315A6F-7724-3D46-84AA-335A70295795}" name="ACTIVIDAD" dataDxfId="95" totalsRowDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{18F811EF-CDDD-DB4A-AA38-F633528B3EA2}" name="RESPONSABLE" dataDxfId="93" totalsRowDxfId="92"/>
-    <tableColumn id="3" xr3:uid="{12BAB512-F0DF-AE43-AB16-88A2C41D1157}" name="ESTADO" dataDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{A3485E03-CCF8-134C-B5A2-953813DDFB7B}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="90" totalsRowDxfId="89" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{43B31EA2-5033-124E-8730-3071676C1780}" name="ID" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{0F148B97-27DE-FB48-8679-E90DD74E6947}" name="VALOR" totalsRowDxfId="92" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{2E315A6F-7724-3D46-84AA-335A70295795}" name="ACTIVIDAD" dataDxfId="91" totalsRowDxfId="90"/>
+    <tableColumn id="6" xr3:uid="{18F811EF-CDDD-DB4A-AA38-F633528B3EA2}" name="RESPONSABLE" dataDxfId="89" totalsRowDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{12BAB512-F0DF-AE43-AB16-88A2C41D1157}" name="ESTADO" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{A3485E03-CCF8-134C-B5A2-953813DDFB7B}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1496,15 +1744,15 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Tabla13475" displayName="Tabla13475" ref="A1:F8" totalsRowCount="1" headerRowDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Tabla13475" displayName="Tabla13475" ref="A1:F8" totalsRowCount="1" headerRowDxfId="77">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B4847248-0602-FF41-ADA7-0593C164551A}" name="ID" dataDxfId="80"/>
-    <tableColumn id="5" xr3:uid="{9570677A-6887-D04B-BC98-FDBF6E642A8E}" name="VALOR" totalsRowDxfId="79" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{F2ACB2B9-3C20-3C4C-86F6-9F569FFCD182}" name="ACTIVIDAD" dataDxfId="78" totalsRowDxfId="77"/>
-    <tableColumn id="6" xr3:uid="{92E380FF-D61D-F04A-83C3-F3A28156C5B7}" name="RESPONSABLE" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{D38B5B8B-4C15-1F44-9B50-D2E36B73D937}" name="ESTADO" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{4229043C-4974-C04E-BCD3-F4185B2BE02C}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="73" totalsRowDxfId="72" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{B4847248-0602-FF41-ADA7-0593C164551A}" name="ID" dataDxfId="76"/>
+    <tableColumn id="5" xr3:uid="{9570677A-6887-D04B-BC98-FDBF6E642A8E}" name="VALOR" totalsRowDxfId="75" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{F2ACB2B9-3C20-3C4C-86F6-9F569FFCD182}" name="ACTIVIDAD" dataDxfId="74" totalsRowDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{92E380FF-D61D-F04A-83C3-F3A28156C5B7}" name="RESPONSABLE" dataDxfId="72" totalsRowDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{D38B5B8B-4C15-1F44-9B50-D2E36B73D937}" name="ESTADO" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{4229043C-4974-C04E-BCD3-F4185B2BE02C}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1513,15 +1761,15 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Tabla1347" displayName="Tabla1347" ref="A1:F8" totalsRowCount="1" headerRowDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Tabla1347" displayName="Tabla1347" ref="A1:F8" totalsRowCount="1" headerRowDxfId="60">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{8530F876-5333-8C42-9B99-E7524B03868D}" name="ID" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{0B425CEF-57FA-0449-9D48-799937F316DA}" name="VALOR" totalsRowDxfId="62" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{A86CCCCE-9767-BA45-8D59-EA4E2B8A125F}" name="ACTIVIDAD" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="6" xr3:uid="{2D321822-E2C3-774D-8799-C0A2CC73F8D9}" name="RESPONSABLE" dataDxfId="59" totalsRowDxfId="58"/>
-    <tableColumn id="3" xr3:uid="{6FFC2B3E-2017-BA44-8965-136231A0E04B}" name="ESTADO" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{A4DFDF0B-96A1-C44C-9DCA-957651D5921A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="56" totalsRowDxfId="55" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{8530F876-5333-8C42-9B99-E7524B03868D}" name="ID" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{0B425CEF-57FA-0449-9D48-799937F316DA}" name="VALOR" totalsRowDxfId="58" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{A86CCCCE-9767-BA45-8D59-EA4E2B8A125F}" name="ACTIVIDAD" dataDxfId="57" totalsRowDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{2D321822-E2C3-774D-8799-C0A2CC73F8D9}" name="RESPONSABLE" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{6FFC2B3E-2017-BA44-8965-136231A0E04B}" name="ESTADO" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{A4DFDF0B-96A1-C44C-9DCA-957651D5921A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1530,15 +1778,15 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Tabla134" displayName="Tabla134" ref="A1:F8" totalsRowCount="1" headerRowDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Tabla134" displayName="Tabla134" ref="A1:F8" totalsRowCount="1" headerRowDxfId="43">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{1F035DC9-1373-3E4C-A3A8-13DBEC76DC82}" name="ID" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{43A5529E-007E-C64C-86CE-8DAB48DE5353}" name="VALOR" totalsRowDxfId="45" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{9A1D5E6B-0F9C-014B-BC79-0CE8E35ABDF2}" name="ACTIVIDAD" dataDxfId="44" totalsRowDxfId="43"/>
-    <tableColumn id="6" xr3:uid="{9DE32ABE-C5F1-6641-97D6-E5E2D7B798CA}" name="RESPONSABLE" dataDxfId="42" totalsRowDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{669DC672-6610-F249-B210-DEC4DB36456B}" name="ESTADO" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{2EC93C66-3A32-2A40-B7A6-F121B89B9430}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{1F035DC9-1373-3E4C-A3A8-13DBEC76DC82}" name="ID" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{43A5529E-007E-C64C-86CE-8DAB48DE5353}" name="VALOR" totalsRowDxfId="41" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{9A1D5E6B-0F9C-014B-BC79-0CE8E35ABDF2}" name="ACTIVIDAD" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="6" xr3:uid="{9DE32ABE-C5F1-6641-97D6-E5E2D7B798CA}" name="RESPONSABLE" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="3" xr3:uid="{669DC672-6610-F249-B210-DEC4DB36456B}" name="ESTADO" dataDxfId="36"/>
+    <tableColumn id="4" xr3:uid="{2EC93C66-3A32-2A40-B7A6-F121B89B9430}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1547,15 +1795,15 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Tabla13" displayName="Tabla13" ref="A1:F8" totalsRowCount="1" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Tabla13" displayName="Tabla13" ref="A1:F8" totalsRowCount="1" headerRowDxfId="26">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{C6E86F07-4CB4-4546-AD18-8C75028994F5}" name="ID" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{DBCD9DEA-ACBA-874C-A22B-59D086F3B877}" name="VALOR" totalsRowDxfId="28" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{D1E5958A-BF8A-BF45-BC61-F88DD4F0DC31}" name="ACTIVIDAD" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{300B975F-DA35-4641-AFFB-C25636AED70A}" name="RESPONSABLE" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{55C19C11-970E-ED48-9E1D-FD413A44DB58}" name="ESTADO" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{F26AE47E-E038-0B42-868B-70E1B4FF0502}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="22" totalsRowDxfId="21" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{C6E86F07-4CB4-4546-AD18-8C75028994F5}" name="ID" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{DBCD9DEA-ACBA-874C-A22B-59D086F3B877}" name="VALOR" totalsRowDxfId="24" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{D1E5958A-BF8A-BF45-BC61-F88DD4F0DC31}" name="ACTIVIDAD" dataDxfId="23" totalsRowDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{300B975F-DA35-4641-AFFB-C25636AED70A}" name="RESPONSABLE" dataDxfId="21" totalsRowDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{55C19C11-970E-ED48-9E1D-FD413A44DB58}" name="ESTADO" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{F26AE47E-E038-0B42-868B-70E1B4FF0502}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1564,15 +1812,15 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{B00B770C-E8F2-CB46-A39B-1F22E5737A8F}" name="ID" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{5618240B-7421-2E49-B85A-37682FDA546C}" name="VALOR" totalsRowDxfId="11" dataCellStyle="Porcentaje"/>
-    <tableColumn id="2" xr3:uid="{FD0BACDA-4B7C-AE4A-B6CC-54F3CF36C08D}" name="ACTIVIDAD" dataDxfId="10" totalsRowDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{FD255310-A28E-5448-BD5D-4F7B55D7AFCB}" name="RESPONSABLE" dataDxfId="8" totalsRowDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{EDB2A1F3-0893-E44D-BCDD-5AACC2B519F8}" name="ESTADO" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{684EEF9A-6840-2141-90A0-69B802ECABA8}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="5" totalsRowDxfId="4" dataCellStyle="Porcentaje">
+    <tableColumn id="1" xr3:uid="{B00B770C-E8F2-CB46-A39B-1F22E5737A8F}" name="ID" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{5618240B-7421-2E49-B85A-37682FDA546C}" name="VALOR" totalsRowDxfId="7" dataCellStyle="Porcentaje"/>
+    <tableColumn id="2" xr3:uid="{FD0BACDA-4B7C-AE4A-B6CC-54F3CF36C08D}" name="ACTIVIDAD" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{FD255310-A28E-5448-BD5D-4F7B55D7AFCB}" name="RESPONSABLE" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{EDB2A1F3-0893-E44D-BCDD-5AACC2B519F8}" name="ESTADO" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{684EEF9A-6840-2141-90A0-69B802ECABA8}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Porcentaje">
       <calculatedColumnFormula>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1846,13 +2094,13 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:I11"/>
+      <selection activeCell="C6" sqref="C6:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="50.83203125" customWidth="1"/>
-    <col min="4" max="4" width="27" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
     <col min="7" max="7" width="19.1640625" customWidth="1"/>
     <col min="8" max="8" width="20.5" customWidth="1"/>
@@ -1872,230 +2120,230 @@
       <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="31"/>
       <c r="I1" s="19" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="23">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="37">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="F2" s="42" t="s">
+      <c r="D2" s="40"/>
+      <c r="F2" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="44"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
       <c r="I2" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="24"/>
-      <c r="B3" s="30"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="27"/>
-      <c r="F3" s="42" t="s">
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="41"/>
+      <c r="F3" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="43"/>
-      <c r="H3" s="44"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
       <c r="I3" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="24"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="27"/>
-      <c r="F4" s="42" t="s">
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="38"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="41"/>
+      <c r="F4" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="43"/>
-      <c r="H4" s="44"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="24"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="27"/>
-      <c r="F5" s="42" t="s">
+    <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="38"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
+      <c r="D5" s="41"/>
+      <c r="F5" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="44"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="25"/>
       <c r="I5" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="24"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="27"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
+    <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="38"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="41"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="25"/>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="34"/>
-      <c r="C7" s="34"/>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="35">
+    <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="42"/>
+    </row>
+    <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="49">
         <v>2</v>
       </c>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="36"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="24"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="38"/>
-      <c r="D9" s="27"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="50"/>
+    </row>
+    <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="38"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="35"/>
+      <c r="D9" s="41"/>
       <c r="F9" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="45" t="s">
+      <c r="G9" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="45"/>
-      <c r="I9" s="45"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="24"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="27"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="26"/>
+    </row>
+    <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="38"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="41"/>
       <c r="F10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="46">
+      <c r="G10" s="27">
         <v>44798</v>
       </c>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+    </row>
+    <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="38"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="41"/>
       <c r="F11" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="24"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="27"/>
-    </row>
-    <row r="13" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="28"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="23">
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+    </row>
+    <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="38"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="41"/>
+    </row>
+    <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="42"/>
+    </row>
+    <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="37">
         <v>3</v>
       </c>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="24"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="27"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="24"/>
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="27"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="24"/>
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="27"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="24"/>
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="27"/>
-    </row>
-    <row r="19" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25"/>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="23">
+      <c r="B14" s="34"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="40"/>
+    </row>
+    <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="38"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
+      <c r="D15" s="41"/>
+    </row>
+    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="38"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="41"/>
+    </row>
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="38"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="35"/>
+      <c r="D17" s="41"/>
+    </row>
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="38"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="41"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="42"/>
+    </row>
+    <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="37">
         <v>4</v>
       </c>
-      <c r="B20" s="40"/>
-      <c r="C20" s="40"/>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="24"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="27"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="24"/>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="27"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="24"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="38"/>
-      <c r="D23" s="27"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="24"/>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="27"/>
-    </row>
-    <row r="25" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="41"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="28"/>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="40"/>
+    </row>
+    <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="38"/>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="41"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="38"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="41"/>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="38"/>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="41"/>
+    </row>
+    <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="38"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="41"/>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="39"/>
+      <c r="B25" s="33"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="42"/>
       <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2104,31 +2352,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="B2:B3"/>
@@ -2145,8 +2368,34 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2720,28 +2969,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="105" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="104" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="100" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="103" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="99" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="102" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="98" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="101" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3025,28 +3274,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="88" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="87" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="85" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="84" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3330,28 +3579,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="71" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="69" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="67" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3635,28 +3884,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="54" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="49" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="51" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="47" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="50" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="45" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3933,28 +4182,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="37" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="33" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4213,28 +4462,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="20" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="7" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="10" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="11" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="12" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SE ANEXA AVANCE DEL MER Y SE ACTUALIZA FORMATO DE SEGUIMIENTO SPRINT 2
</commit_message>
<xml_diff>
--- a/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
+++ b/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/SPRINT1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B80E128-2EEB-8B44-806C-30611974EE35}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B266F811-ADD2-7F44-9696-F95D338C85AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME SPRINT" sheetId="12" r:id="rId1"/>
@@ -609,7 +609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -655,49 +655,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -740,6 +699,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2093,8 +2100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30953C18-D402-474E-9F52-63E7C872EAD8}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2120,230 +2127,230 @@
       <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="43"/>
       <c r="I1" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="37">
+      <c r="A2" s="22">
         <v>1</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="25"/>
+      <c r="F2" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="24"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="2" t="s">
+      <c r="G2" s="45"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="47" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="46"/>
-      <c r="D3" s="41"/>
-      <c r="F3" s="23" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="26"/>
+      <c r="F3" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="24"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="2" t="s">
+      <c r="G3" s="45"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="38"/>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="41"/>
-      <c r="F4" s="23" t="s">
+      <c r="A4" s="23"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="26"/>
+      <c r="F4" s="44" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="24"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="2" t="s">
+      <c r="G4" s="45"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="47" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="41"/>
-      <c r="F5" s="23" t="s">
+      <c r="A5" s="23"/>
+      <c r="B5" s="29"/>
+      <c r="C5" s="29"/>
+      <c r="D5" s="26"/>
+      <c r="F5" s="44" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="24"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="2" t="s">
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="41"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="2"/>
+      <c r="A6" s="23"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="26"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="45"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="42"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="27"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49">
+      <c r="A8" s="34">
         <v>2</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="36"/>
-      <c r="D8" s="50"/>
+      <c r="D8" s="35"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="41"/>
-      <c r="F9" s="21" t="s">
+      <c r="A9" s="23"/>
+      <c r="B9" s="37"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="26"/>
+      <c r="F9" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="26" t="s">
+      <c r="G9" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38"/>
-      <c r="B10" s="32"/>
-      <c r="C10" s="32"/>
-      <c r="D10" s="41"/>
-      <c r="F10" s="21" t="s">
+      <c r="A10" s="23"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="26"/>
+      <c r="F10" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="27">
+      <c r="G10" s="49">
         <v>44798</v>
       </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="41"/>
-      <c r="F11" s="21" t="s">
+      <c r="A11" s="23"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="26"/>
+      <c r="F11" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="50" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
+      <c r="H11" s="50"/>
+      <c r="I11" s="50"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="41"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
-      <c r="B13" s="33"/>
-      <c r="C13" s="33"/>
-      <c r="D13" s="42"/>
+      <c r="A13" s="24"/>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="37">
+      <c r="A14" s="22">
         <v>3</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="40"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+      <c r="D14" s="25"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="41"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="41"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="26"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="35"/>
-      <c r="D17" s="41"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="38"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="41"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
-      <c r="B19" s="33"/>
-      <c r="C19" s="33"/>
-      <c r="D19" s="42"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="37">
+      <c r="A20" s="22">
         <v>4</v>
       </c>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="40"/>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="38"/>
-      <c r="B21" s="35"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="41"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="37"/>
+      <c r="C21" s="37"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
-      <c r="D22" s="41"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="38"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="B23" s="35"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="41"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="37"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="41"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="39"/>
-      <c r="B25" s="33"/>
-      <c r="C25" s="33"/>
-      <c r="D25" s="42"/>
+      <c r="A25" s="24"/>
+      <c r="B25" s="40"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="27"/>
       <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2352,6 +2359,31 @@
     </row>
   </sheetData>
   <mergeCells count="41">
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="B2:B3"/>
@@ -2368,31 +2400,6 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2403,7 +2410,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F45049-B0C9-8441-BE8F-F70E663206EB}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -2599,13 +2606,13 @@
         <f>COUNTIF(Tabla1347568[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2617,7 +2624,7 @@
         <f>COUNTIF(Tabla1347568[ESTADO],"VERIFICAR")</f>
         <v>1</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="20" t="s">
@@ -2635,7 +2642,7 @@
         <f>COUNTIF(Tabla1347568[ESTADO],"HECHO")</f>
         <v>5</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="20" t="s">
@@ -2646,7 +2653,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="20" t="s">
@@ -2904,13 +2911,13 @@
         <f>COUNTIF(Tabla134756[ESTADO],"HACIENDO")</f>
         <v>2</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2922,7 +2929,7 @@
         <f>COUNTIF(Tabla134756[ESTADO],"VERIFICAR")</f>
         <v>1</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -2940,7 +2947,7 @@
         <f>COUNTIF(Tabla134756[ESTADO],"HECHO")</f>
         <v>3</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -2951,7 +2958,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3209,13 +3216,13 @@
         <f>COUNTIF(Tabla13475[ESTADO],"HACIENDO")</f>
         <v>1</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3227,7 +3234,7 @@
         <f>COUNTIF(Tabla13475[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3245,7 +3252,7 @@
         <f>COUNTIF(Tabla13475[ESTADO],"HECHO")</f>
         <v>2</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3256,7 +3263,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3514,13 +3521,13 @@
         <f>COUNTIF(Tabla1347[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3532,7 +3539,7 @@
         <f>COUNTIF(Tabla1347[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3550,7 +3557,7 @@
         <f>COUNTIF(Tabla1347[ESTADO],"HECHO")</f>
         <v>1</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3561,7 +3568,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -3819,13 +3826,13 @@
         <f>COUNTIF(Tabla134[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3837,7 +3844,7 @@
         <f>COUNTIF(Tabla134[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -3855,7 +3862,7 @@
         <f>COUNTIF(Tabla134[ESTADO],"HECHO")</f>
         <v>1</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -3866,7 +3873,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -4123,13 +4130,13 @@
         <f>COUNTIF(Tabla13[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4141,7 +4148,7 @@
         <f>COUNTIF(Tabla13[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -4159,7 +4166,7 @@
         <f>COUNTIF(Tabla13[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -4170,7 +4177,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -4399,13 +4406,13 @@
         <f>COUNTIF(Tabla1[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
-      <c r="F12" s="22">
+      <c r="F12" s="21">
         <v>1</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -4417,7 +4424,7 @@
         <f>COUNTIF(Tabla1[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="21">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="s">
@@ -4435,7 +4442,7 @@
         <f>COUNTIF(Tabla1[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
-      <c r="F14" s="22">
+      <c r="F14" s="21">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="s">
@@ -4446,7 +4453,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="22">
+      <c r="F15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="s">

</xml_diff>

<commit_message>
SE MODIFICAN MODELO CONCEPTUAL Y MER, SE ANEXA FORMATO DE SEGUIMIENTO GENERAL DE ACTIVIDADES
</commit_message>
<xml_diff>
--- a/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
+++ b/SPRINT1/FORMATO SEGUIMIENTO-SPRINT1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/BrandonMedina/Documents/ACADEMICO/MISION TIC/DESARROLLO DE SOFTWARE/MINTIC-84-02/SPRINT1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B266F811-ADD2-7F44-9696-F95D338C85AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5634598E-E74B-FA41-84F2-A47369D66DE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INFORME SPRINT" sheetId="12" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="PLANEACION 21-08-2022" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="55">
   <si>
     <t>HACER</t>
   </si>
@@ -207,6 +208,9 @@
   </si>
   <si>
     <t>Se distribuye la actividad asignada de ese miembro entre todos los miembros del equipo</t>
+  </si>
+  <si>
+    <t>ACTIVIDADES POSPUESTAS</t>
   </si>
 </sst>
 </file>
@@ -270,7 +274,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,6 +323,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="21">
     <border>
@@ -609,7 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,6 +668,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -699,54 +758,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1717,7 +1728,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DAF9B008-E008-A544-84D7-8559DC8E169A}" name="Tabla1347568" displayName="Tabla1347568" ref="A1:F8" totalsRowCount="1" headerRowDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DAF9B008-E008-A544-84D7-8559DC8E169A}" name="Reunion5" displayName="Reunion5" ref="A1:F8" totalsRowCount="1" headerRowDxfId="111">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{5C096F99-9B91-DE40-878E-814BDFEB9846}" name="ID" dataDxfId="110"/>
@@ -1726,7 +1737,7 @@
     <tableColumn id="6" xr3:uid="{D5B7DF44-BD95-454D-B6F6-6601063DE794}" name="RESPONSABLE" dataDxfId="106" totalsRowDxfId="105"/>
     <tableColumn id="3" xr3:uid="{3FAAD558-904B-DD40-920C-627F98A8C8D5}" name="ESTADO" dataDxfId="104"/>
     <tableColumn id="4" xr3:uid="{ED810AD6-1A4E-FF44-ADA4-0F9B58BF457A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="103" totalsRowDxfId="102" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1734,7 +1745,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Tabla134756" displayName="Tabla134756" ref="A1:F8" totalsRowCount="1" headerRowDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DAA0380F-4B90-4348-B2FF-E65E4C0E83C3}" name="Reunion4" displayName="Reunion4" ref="A1:F8" totalsRowCount="1" headerRowDxfId="94">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{43B31EA2-5033-124E-8730-3071676C1780}" name="ID" dataDxfId="93"/>
@@ -1743,7 +1754,7 @@
     <tableColumn id="6" xr3:uid="{18F811EF-CDDD-DB4A-AA38-F633528B3EA2}" name="RESPONSABLE" dataDxfId="89" totalsRowDxfId="88"/>
     <tableColumn id="3" xr3:uid="{12BAB512-F0DF-AE43-AB16-88A2C41D1157}" name="ESTADO" dataDxfId="87"/>
     <tableColumn id="4" xr3:uid="{A3485E03-CCF8-134C-B5A2-953813DDFB7B}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="86" totalsRowDxfId="85" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1751,7 +1762,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Tabla13475" displayName="Tabla13475" ref="A1:F8" totalsRowCount="1" headerRowDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{57A39197-0EB7-7144-8D73-78264AB813B5}" name="Reunion3" displayName="Reunion3" ref="A1:F8" totalsRowCount="1" headerRowDxfId="77">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B4847248-0602-FF41-ADA7-0593C164551A}" name="ID" dataDxfId="76"/>
@@ -1760,7 +1771,7 @@
     <tableColumn id="6" xr3:uid="{92E380FF-D61D-F04A-83C3-F3A28156C5B7}" name="RESPONSABLE" dataDxfId="72" totalsRowDxfId="71"/>
     <tableColumn id="3" xr3:uid="{D38B5B8B-4C15-1F44-9B50-D2E36B73D937}" name="ESTADO" dataDxfId="70"/>
     <tableColumn id="4" xr3:uid="{4229043C-4974-C04E-BCD3-F4185B2BE02C}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1768,7 +1779,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Tabla1347" displayName="Tabla1347" ref="A1:F8" totalsRowCount="1" headerRowDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{D7E5A0F1-F6B5-9C4A-B5AF-7F17798D8F2E}" name="Reunion2" displayName="Reunion2" ref="A1:F8" totalsRowCount="1" headerRowDxfId="60">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8530F876-5333-8C42-9B99-E7524B03868D}" name="ID" dataDxfId="59"/>
@@ -1777,7 +1788,7 @@
     <tableColumn id="6" xr3:uid="{2D321822-E2C3-774D-8799-C0A2CC73F8D9}" name="RESPONSABLE" dataDxfId="55" totalsRowDxfId="54"/>
     <tableColumn id="3" xr3:uid="{6FFC2B3E-2017-BA44-8965-136231A0E04B}" name="ESTADO" dataDxfId="53"/>
     <tableColumn id="4" xr3:uid="{A4DFDF0B-96A1-C44C-9DCA-957651D5921A}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="52" totalsRowDxfId="51" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1785,7 +1796,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Tabla134" displayName="Tabla134" ref="A1:F8" totalsRowCount="1" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{41D43311-9DED-5545-8A36-F8DE9AD321E8}" name="Reunion1" displayName="Reunion1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="43">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{1F035DC9-1373-3E4C-A3A8-13DBEC76DC82}" name="ID" dataDxfId="42"/>
@@ -1794,7 +1805,7 @@
     <tableColumn id="6" xr3:uid="{9DE32ABE-C5F1-6641-97D6-E5E2D7B798CA}" name="RESPONSABLE" dataDxfId="38" totalsRowDxfId="37"/>
     <tableColumn id="3" xr3:uid="{669DC672-6610-F249-B210-DEC4DB36456B}" name="ESTADO" dataDxfId="36"/>
     <tableColumn id="4" xr3:uid="{2EC93C66-3A32-2A40-B7A6-F121B89B9430}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="35" totalsRowDxfId="34" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1802,7 +1813,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Tabla13" displayName="Tabla13" ref="A1:F8" totalsRowCount="1" headerRowDxfId="26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D1A28B4D-94D1-FB40-988C-D0AD4A4C55EF}" name="Distribucion" displayName="Distribucion" ref="A1:F8" totalsRowCount="1" headerRowDxfId="26">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C6E86F07-4CB4-4546-AD18-8C75028994F5}" name="ID" dataDxfId="25"/>
@@ -1811,7 +1822,7 @@
     <tableColumn id="6" xr3:uid="{300B975F-DA35-4641-AFFB-C25636AED70A}" name="RESPONSABLE" dataDxfId="21" totalsRowDxfId="20"/>
     <tableColumn id="3" xr3:uid="{55C19C11-970E-ED48-9E1D-FD413A44DB58}" name="ESTADO" dataDxfId="19"/>
     <tableColumn id="4" xr3:uid="{F26AE47E-E038-0B42-868B-70E1B4FF0502}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="18" totalsRowDxfId="17" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1819,7 +1830,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Tabla1" displayName="Tabla1" ref="A1:F8" totalsRowCount="1" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41261913-023D-9742-9092-C234634FC4AA}" name="Planeacion" displayName="Planeacion" ref="A1:F8" totalsRowCount="1" headerRowDxfId="9">
   <autoFilter ref="A1:F7" xr:uid="{C6771560-9D89-3142-9F9C-47C6E5E14ADD}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{B00B770C-E8F2-CB46-A39B-1F22E5737A8F}" name="ID" dataDxfId="8"/>
@@ -1828,7 +1839,7 @@
     <tableColumn id="6" xr3:uid="{FD255310-A28E-5448-BD5D-4F7B55D7AFCB}" name="RESPONSABLE" dataDxfId="4" totalsRowDxfId="3"/>
     <tableColumn id="3" xr3:uid="{EDB2A1F3-0893-E44D-BCDD-5AACC2B519F8}" name="ESTADO" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{684EEF9A-6840-2141-90A0-69B802ECABA8}" name="PROGRESO" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0" dataCellStyle="Porcentaje">
-      <calculatedColumnFormula>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
+      <calculatedColumnFormula>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2100,7 +2111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30953C18-D402-474E-9F52-63E7C872EAD8}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F5" sqref="F5:H5"/>
     </sheetView>
   </sheetViews>
@@ -2127,230 +2138,230 @@
       <c r="D1" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="43"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="33"/>
       <c r="I1" s="19" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+      <c r="A2" s="39">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="F2" s="44" t="s">
+      <c r="D2" s="42"/>
+      <c r="F2" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47" t="s">
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="23"/>
-      <c r="B3" s="29"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="26"/>
-      <c r="F3" s="44" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="43"/>
+      <c r="F3" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="G3" s="45"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47" t="s">
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="23"/>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="26"/>
-      <c r="F4" s="44" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="43"/>
+      <c r="F4" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="45"/>
-      <c r="H4" s="46"/>
-      <c r="I4" s="47" t="s">
+      <c r="G4" s="26"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="23"/>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
-      <c r="D5" s="26"/>
-      <c r="F5" s="44" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="43"/>
+      <c r="F5" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="47" t="s">
+      <c r="G5" s="26"/>
+      <c r="H5" s="27"/>
+      <c r="I5" s="22" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="23"/>
-      <c r="B6" s="32"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="26"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="46"/>
-      <c r="I6" s="47"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="43"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="22"/>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="33"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="27"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="44"/>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="34">
+      <c r="A8" s="51">
         <v>2</v>
       </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
-      <c r="D8" s="35"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="52"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
+      <c r="A9" s="40"/>
       <c r="B9" s="37"/>
       <c r="C9" s="37"/>
-      <c r="D9" s="26"/>
-      <c r="F9" s="51" t="s">
+      <c r="D9" s="43"/>
+      <c r="F9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="48" t="s">
+      <c r="G9" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="23"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="26"/>
-      <c r="F10" s="51" t="s">
+      <c r="A10" s="40"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="43"/>
+      <c r="F10" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G10" s="49">
+      <c r="G10" s="29">
         <v>44798</v>
       </c>
-      <c r="H10" s="49"/>
-      <c r="I10" s="49"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="23"/>
+      <c r="A11" s="40"/>
       <c r="B11" s="37"/>
       <c r="C11" s="37"/>
-      <c r="D11" s="26"/>
-      <c r="F11" s="51" t="s">
+      <c r="D11" s="43"/>
+      <c r="F11" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="50" t="s">
+      <c r="G11" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="50"/>
-      <c r="I11" s="50"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="38"/>
-      <c r="C12" s="38"/>
-      <c r="D12" s="26"/>
+      <c r="A12" s="40"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="43"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="27"/>
+      <c r="A13" s="41"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="44"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
+      <c r="A14" s="39">
         <v>3</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="25"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="42"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
+      <c r="A15" s="40"/>
       <c r="B15" s="37"/>
       <c r="C15" s="37"/>
-      <c r="D15" s="26"/>
+      <c r="D15" s="43"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="26"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="43"/>
     </row>
     <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
+      <c r="A17" s="40"/>
       <c r="B17" s="37"/>
       <c r="C17" s="37"/>
-      <c r="D17" s="26"/>
+      <c r="D17" s="43"/>
     </row>
     <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="26"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="43"/>
     </row>
     <row r="19" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="24"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="27"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="44"/>
     </row>
     <row r="20" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="22">
+      <c r="A20" s="39">
         <v>4</v>
       </c>
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="25"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="42"/>
     </row>
     <row r="21" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
+      <c r="A21" s="40"/>
       <c r="B21" s="37"/>
       <c r="C21" s="37"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="43"/>
     </row>
     <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="38"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="26"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="34"/>
+      <c r="C22" s="34"/>
+      <c r="D22" s="43"/>
     </row>
     <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
+      <c r="A23" s="40"/>
       <c r="B23" s="37"/>
       <c r="C23" s="37"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="43"/>
     </row>
     <row r="24" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="26"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="34"/>
+      <c r="C24" s="34"/>
+      <c r="D24" s="43"/>
     </row>
     <row r="25" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24"/>
-      <c r="B25" s="40"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="27"/>
+      <c r="A25" s="41"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="44"/>
       <c r="F25" s="1" t="s">
         <v>14</v>
       </c>
@@ -2359,31 +2370,6 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="F1:H1"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C12:C13"/>
     <mergeCell ref="A20:A25"/>
     <mergeCell ref="D20:D25"/>
     <mergeCell ref="B2:B3"/>
@@ -2400,6 +2386,31 @@
     <mergeCell ref="D14:D19"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2408,6 +2419,630 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36F45049-B0C9-8441-BE8F-F70E663206EB}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6">
+        <f>IF(Reunion5[[#This Row],[ESTADO]]="HECHO",Reunion5[[#This Row],[VALOR]]," ")</f>
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="7">
+        <f>SUBTOTAL(109,Reunion5[PROGRESO])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <f>COUNTIF(Reunion5[ESTADO],"HACER")</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <f>COUNTIF(Reunion5[ESTADO],"HACIENDO")</f>
+        <v>0</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <f>COUNTIF(Reunion5[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
+      </c>
+      <c r="F13" s="21">
+        <v>2</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3">
+        <f>COUNTIF(Reunion5[ESTADO],"HECHO")</f>
+        <v>6</v>
+      </c>
+      <c r="F14" s="21">
+        <v>3</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Reunion5[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21">
+        <v>4</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="117" priority="5" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="6" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="115" priority="7" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="113" priority="2" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="112" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{173F3A64-8499-FE46-8D27-CA94C26E5A89}">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{72532A5C-9CE8-FE40-826C-5A123CFDB9D6}">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A8DC1C-B48E-3D45-8831-0A62DF6933FD}">
+  <dimension ref="A1:H17"/>
+  <sheetViews>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="6.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.83203125" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" customWidth="1"/>
+    <col min="9" max="10" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="6">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0.05</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="6">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="6">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="str">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="H6" s="7"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="str">
+        <f>IF(Reunion4[[#This Row],[ESTADO]]="HECHO",Reunion4[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="8"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="F8" s="7">
+        <f>SUBTOTAL(109,Reunion4[PROGRESO])</f>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3">
+        <f>COUNTIF(Reunion4[ESTADO],"HACER")</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C12" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="3">
+        <f>COUNTIF(Reunion4[ESTADO],"HACIENDO")</f>
+        <v>2</v>
+      </c>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C13" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3">
+        <f>COUNTIF(Reunion4[ESTADO],"VERIFICAR")</f>
+        <v>1</v>
+      </c>
+      <c r="F13" s="21">
+        <v>2</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="3">
+        <f>COUNTIF(Reunion4[ESTADO],"HECHO")</f>
+        <v>3</v>
+      </c>
+      <c r="F14" s="21">
+        <v>3</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Reunion4[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="21">
+        <v>4</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E2:E7">
+    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+      <formula>($E2="VERIFICAR")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="100" priority="5" stopIfTrue="1">
+      <formula>($E2="HECHO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="99" priority="6" stopIfTrue="1">
+      <formula>($E2="HACIENDO")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="98" priority="7" stopIfTrue="1">
+      <formula>($E2="HACER")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="greaterThan">
+      <formula>0.67</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="between">
+      <formula>0.34</formula>
+      <formula>0.66</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="lessThan">
+      <formula>0.33</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{84260B45-8E3A-2F4C-AA08-81743E5FB103}">
+      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{B73ED223-9B85-AF47-B17F-B38AAC6FB6A9}">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A12336-19D1-7A49-A729-A680FE050C77}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
@@ -2461,7 +3096,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="6">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
         <v>0.1</v>
       </c>
     </row>
@@ -2482,7 +3117,7 @@
         <v>2</v>
       </c>
       <c r="F3" s="6">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
         <v>0.05</v>
       </c>
     </row>
@@ -2500,11 +3135,11 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
-        <v>0.4</v>
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2521,11 +3156,11 @@
         <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5" s="6">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
-        <v>0.1</v>
+        <v>0</v>
+      </c>
+      <c r="F5" s="6" t="str">
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -2542,11 +3177,11 @@
         <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="6">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
-        <v>0.2</v>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6" t="str">
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -2564,10 +3199,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="str">
-        <f>IF(Tabla1347568[[#This Row],[ESTADO]]="HECHO",Tabla1347568[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion3[[#This Row],[ESTADO]]="HECHO",Reunion3[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2576,8 +3211,8 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla1347568[PROGRESO])</f>
-        <v>0.85000000000000009</v>
+        <f>SUBTOTAL(109,Reunion3[PROGRESO])</f>
+        <v>0.15000000000000002</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2585,8 +3220,8 @@
         <v>21</v>
       </c>
       <c r="D11" s="3">
-        <f>COUNTIF(Tabla1347568[ESTADO],"HACER")</f>
-        <v>0</v>
+        <f>COUNTIF(Reunion3[ESTADO],"HACER")</f>
+        <v>3</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>28</v>
@@ -2603,8 +3238,8 @@
         <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f>COUNTIF(Tabla1347568[ESTADO],"HACIENDO")</f>
-        <v>0</v>
+        <f>COUNTIF(Reunion3[ESTADO],"HACIENDO")</f>
+        <v>1</v>
       </c>
       <c r="F12" s="21">
         <v>1</v>
@@ -2621,16 +3256,16 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <f>COUNTIF(Tabla1347568[ESTADO],"VERIFICAR")</f>
-        <v>1</v>
+        <f>COUNTIF(Reunion3[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
       </c>
       <c r="F13" s="21">
         <v>2</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H13" s="20" t="s">
+      <c r="H13" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2639,27 +3274,34 @@
         <v>23</v>
       </c>
       <c r="D14" s="3">
-        <f>COUNTIF(Tabla1347568[ESTADO],"HECHO")</f>
-        <v>5</v>
+        <f>COUNTIF(Reunion3[ESTADO],"HECHO")</f>
+        <v>2</v>
       </c>
       <c r="F14" s="21">
         <v>3</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="20" t="s">
+      <c r="H14" s="2" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Reunion3[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="21">
         <v>4</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="H15" s="20" t="s">
+      <c r="H15" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2671,36 +3313,36 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="118" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="84" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="117" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="83" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="116" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="82" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="115" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="81" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="114" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="79" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{173F3A64-8499-FE46-8D27-CA94C26E5A89}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{BDF37FF0-D80D-9745-8E13-7828AD712828}">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{72532A5C-9CE8-FE40-826C-5A123CFDB9D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{BCA0D857-6F06-5F4B-902E-679BAAC0A35F}">
       <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2711,12 +3353,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A8DC1C-B48E-3D45-8831-0A62DF6933FD}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA48102-9501-E841-A6C2-864B0ECAAC64}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E7" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2766,7 +3408,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="6">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
         <v>0.1</v>
       </c>
     </row>
@@ -2784,11 +3426,11 @@
         <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -2805,11 +3447,11 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="6">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
-        <v>0.4</v>
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="str">
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
@@ -2826,10 +3468,10 @@
         <v>33</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" s="6" t="str">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2847,10 +3489,10 @@
         <v>30</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="6" t="str">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="7"/>
@@ -2869,10 +3511,10 @@
         <v>31</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F7" s="6" t="str">
-        <f>IF(Tabla134756[[#This Row],[ESTADO]]="HECHO",Tabla134756[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion2[[#This Row],[ESTADO]]="HECHO",Reunion2[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -2881,8 +3523,8 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla134756[PROGRESO])</f>
-        <v>0.55000000000000004</v>
+        <f>SUBTOTAL(109,Reunion2[PROGRESO])</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -2890,8 +3532,8 @@
         <v>21</v>
       </c>
       <c r="D11" s="3">
-        <f>COUNTIF(Tabla134756[ESTADO],"HACER")</f>
-        <v>0</v>
+        <f>COUNTIF(Reunion2[ESTADO],"HACER")</f>
+        <v>5</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>28</v>
@@ -2908,8 +3550,8 @@
         <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f>COUNTIF(Tabla134756[ESTADO],"HACIENDO")</f>
-        <v>2</v>
+        <f>COUNTIF(Reunion2[ESTADO],"HACIENDO")</f>
+        <v>0</v>
       </c>
       <c r="F12" s="21">
         <v>1</v>
@@ -2926,8 +3568,8 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <f>COUNTIF(Tabla134756[ESTADO],"VERIFICAR")</f>
-        <v>1</v>
+        <f>COUNTIF(Reunion2[ESTADO],"VERIFICAR")</f>
+        <v>0</v>
       </c>
       <c r="F13" s="21">
         <v>2</v>
@@ -2944,8 +3586,8 @@
         <v>23</v>
       </c>
       <c r="D14" s="3">
-        <f>COUNTIF(Tabla134756[ESTADO],"HECHO")</f>
-        <v>3</v>
+        <f>COUNTIF(Reunion2[ESTADO],"HECHO")</f>
+        <v>1</v>
       </c>
       <c r="F14" s="21">
         <v>3</v>
@@ -2958,6 +3600,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Reunion2[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="21">
         <v>4</v>
       </c>
@@ -2976,37 +3625,37 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="101" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="67" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="66" priority="5" stopIfTrue="1">
       <formula>($E2="HECHO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="99" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="65" priority="6" stopIfTrue="1">
       <formula>($E2="HACIENDO")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
       <formula>($E2="HACER")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="97" priority="1" stopIfTrue="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="1" stopIfTrue="1" operator="greaterThan">
       <formula>0.67</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="62" priority="2" stopIfTrue="1" operator="between">
       <formula>0.34</formula>
       <formula>0.66</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="3" stopIfTrue="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="3" stopIfTrue="1" operator="lessThan">
       <formula>0.33</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{84260B45-8E3A-2F4C-AA08-81743E5FB103}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{79AA00C3-40E6-3E45-92B6-8A367E279B74}">
       <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{B73ED223-9B85-AF47-B17F-B38AAC6FB6A9}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{2DBA36AE-7F85-6F4F-89E0-108C93C10193}">
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3016,12 +3665,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53A12336-19D1-7A49-A729-A680FE050C77}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FEBE19-1B7C-E447-8CE1-7FE68E40E356}">
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3071,7 +3720,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="6">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
         <v>0.1</v>
       </c>
     </row>
@@ -3089,11 +3738,11 @@
         <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="6">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
-        <v>0.05</v>
+        <v>0</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
+        <v xml:space="preserve"> </v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -3110,10 +3759,10 @@
         <v>29</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F4" s="6" t="str">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3134,7 +3783,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="6" t="str">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3155,7 +3804,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6" t="str">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="7"/>
@@ -3177,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6" t="str">
-        <f>IF(Tabla13475[[#This Row],[ESTADO]]="HECHO",Tabla13475[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Reunion1[[#This Row],[ESTADO]]="HECHO",Reunion1[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -3186,8 +3835,8 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla13475[PROGRESO])</f>
-        <v>0.15000000000000002</v>
+        <f>SUBTOTAL(109,Reunion1[PROGRESO])</f>
+        <v>0.1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
@@ -3195,8 +3844,8 @@
         <v>21</v>
       </c>
       <c r="D11" s="3">
-        <f>COUNTIF(Tabla13475[ESTADO],"HACER")</f>
-        <v>3</v>
+        <f>COUNTIF(Reunion1[ESTADO],"HACER")</f>
+        <v>5</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>28</v>
@@ -3213,8 +3862,8 @@
         <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f>COUNTIF(Tabla13475[ESTADO],"HACIENDO")</f>
-        <v>1</v>
+        <f>COUNTIF(Reunion1[ESTADO],"HACIENDO")</f>
+        <v>0</v>
       </c>
       <c r="F12" s="21">
         <v>1</v>
@@ -3231,7 +3880,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <f>COUNTIF(Tabla13475[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Reunion1[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="F13" s="21">
@@ -3249,8 +3898,8 @@
         <v>23</v>
       </c>
       <c r="D14" s="3">
-        <f>COUNTIF(Tabla13475[ESTADO],"HECHO")</f>
-        <v>2</v>
+        <f>COUNTIF(Reunion1[ESTADO],"HECHO")</f>
+        <v>1</v>
       </c>
       <c r="F14" s="21">
         <v>3</v>
@@ -3263,6 +3912,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Reunion1[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="21">
         <v>4</v>
       </c>
@@ -3281,616 +3937,6 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="84" priority="4" stopIfTrue="1">
-      <formula>($E2="VERIFICAR")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="83" priority="5" stopIfTrue="1">
-      <formula>($E2="HECHO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="82" priority="6" stopIfTrue="1">
-      <formula>($E2="HACIENDO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="81" priority="7" stopIfTrue="1">
-      <formula>($E2="HACER")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="80" priority="1" stopIfTrue="1" operator="greaterThan">
-      <formula>0.67</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="2" stopIfTrue="1" operator="between">
-      <formula>0.34</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="3" stopIfTrue="1" operator="lessThan">
-      <formula>0.33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{BDF37FF0-D80D-9745-8E13-7828AD712828}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{BCA0D857-6F06-5F4B-902E-679BAAC0A35F}">
-      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FA48102-9501-E841-A6C2-864B0ECAAC64}">
-  <dimension ref="A1:H17"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="str">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="str">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="str">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="str">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="str">
-        <f>IF(Tabla1347[[#This Row],[ESTADO]]="HECHO",Tabla1347[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla1347[PROGRESO])</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3">
-        <f>COUNTIF(Tabla1347[ESTADO],"HACER")</f>
-        <v>5</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3">
-        <f>COUNTIF(Tabla1347[ESTADO],"HACIENDO")</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3">
-        <f>COUNTIF(Tabla1347[ESTADO],"VERIFICAR")</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="21">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3">
-        <f>COUNTIF(Tabla1347[ESTADO],"HECHO")</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="21">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="21">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E2:E7">
-    <cfRule type="expression" dxfId="67" priority="4" stopIfTrue="1">
-      <formula>($E2="VERIFICAR")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="66" priority="5" stopIfTrue="1">
-      <formula>($E2="HECHO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="65" priority="6" stopIfTrue="1">
-      <formula>($E2="HACIENDO")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="64" priority="7" stopIfTrue="1">
-      <formula>($E2="HACER")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="63" priority="1" stopIfTrue="1" operator="greaterThan">
-      <formula>0.67</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="2" stopIfTrue="1" operator="between">
-      <formula>0.34</formula>
-      <formula>0.66</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="3" stopIfTrue="1" operator="lessThan">
-      <formula>0.33</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{79AA00C3-40E6-3E45-92B6-8A367E279B74}">
-      <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{2DBA36AE-7F85-6F4F-89E0-108C93C10193}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6FEBE19-1B7C-E447-8CE1-7FE68E40E356}">
-  <dimension ref="A1:H17"/>
-  <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="6.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
-    <col min="5" max="6" width="13.83203125" customWidth="1"/>
-    <col min="7" max="7" width="24.83203125" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="10" width="10.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="6">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6" t="str">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="str">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6" t="str">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6">
-        <v>0.2</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="6" t="str">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H6" s="7"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="6" t="str">
-        <f>IF(Tabla134[[#This Row],[ESTADO]]="HECHO",Tabla134[[#This Row],[VALOR]]," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla134[PROGRESO])</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C11" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3">
-        <f>COUNTIF(Tabla134[ESTADO],"HACER")</f>
-        <v>5</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="17" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C12" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="3">
-        <f>COUNTIF(Tabla134[ESTADO],"HACIENDO")</f>
-        <v>0</v>
-      </c>
-      <c r="F12" s="21">
-        <v>1</v>
-      </c>
-      <c r="G12" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C13" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="3">
-        <f>COUNTIF(Tabla134[ESTADO],"VERIFICAR")</f>
-        <v>0</v>
-      </c>
-      <c r="F13" s="21">
-        <v>2</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="C14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="3">
-        <f>COUNTIF(Tabla134[ESTADO],"HECHO")</f>
-        <v>1</v>
-      </c>
-      <c r="F14" s="21">
-        <v>3</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="F15" s="21">
-        <v>4</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="E2:E7">
     <cfRule type="expression" dxfId="50" priority="4" stopIfTrue="1">
       <formula>($E2="VERIFICAR")</formula>
     </cfRule>
@@ -3918,7 +3964,7 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{4A04957C-324B-DB45-85A3-FF861B8AD7A4}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{91C4C282-AB21-F444-BCB2-88768A8413D7}">
       <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
@@ -3936,7 +3982,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E3" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3985,7 +4031,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4006,7 +4052,7 @@
         <v>0</v>
       </c>
       <c r="F3" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4027,7 +4073,7 @@
         <v>0</v>
       </c>
       <c r="F4" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4048,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4069,7 +4115,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="7"/>
@@ -4091,7 +4137,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6" t="str">
-        <f>IF(Tabla13[[#This Row],[ESTADO]]="HECHO",Tabla13[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Distribucion[[#This Row],[ESTADO]]="HECHO",Distribucion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4100,7 +4146,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla13[PROGRESO])</f>
+        <f>SUBTOTAL(109,Distribucion[PROGRESO])</f>
         <v>0</v>
       </c>
     </row>
@@ -4109,7 +4155,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="3">
-        <f>COUNTIF(Tabla13[ESTADO],"HACER")</f>
+        <f>COUNTIF(Distribucion[ESTADO],"HACER")</f>
         <v>6</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -4127,7 +4173,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f>COUNTIF(Tabla13[ESTADO],"HACIENDO")</f>
+        <f>COUNTIF(Distribucion[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
       <c r="F12" s="21">
@@ -4145,7 +4191,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <f>COUNTIF(Tabla13[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Distribucion[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="F13" s="21">
@@ -4163,7 +4209,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="3">
-        <f>COUNTIF(Tabla13[ESTADO],"HECHO")</f>
+        <f>COUNTIF(Distribucion[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
       <c r="F14" s="21">
@@ -4177,6 +4223,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Distribucion[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="21">
         <v>4</v>
       </c>
@@ -4219,7 +4272,7 @@
       <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{4F90FE47-B0C7-BD4D-8030-1D92CAC580FC}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4234,7 +4287,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="E2" sqref="E2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4281,7 +4334,7 @@
       <c r="D2" s="4"/>
       <c r="E2" s="5"/>
       <c r="F2" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4298,7 +4351,7 @@
       <c r="D3" s="4"/>
       <c r="E3" s="5"/>
       <c r="F3" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4315,7 +4368,7 @@
       <c r="D4" s="4"/>
       <c r="E4" s="5"/>
       <c r="F4" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4332,7 +4385,7 @@
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
       <c r="F5" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4349,7 +4402,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="5"/>
       <c r="F6" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="H6" s="7"/>
@@ -4367,7 +4420,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6" t="str">
-        <f>IF(Tabla1[[#This Row],[ESTADO]]="HECHO",Tabla1[[#This Row],[VALOR]]," ")</f>
+        <f>IF(Planeacion[[#This Row],[ESTADO]]="HECHO",Planeacion[[#This Row],[VALOR]]," ")</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
@@ -4376,7 +4429,7 @@
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
       <c r="F8" s="7">
-        <f>SUBTOTAL(109,Tabla1[PROGRESO])</f>
+        <f>SUBTOTAL(109,Planeacion[PROGRESO])</f>
         <v>0</v>
       </c>
     </row>
@@ -4385,7 +4438,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="3">
-        <f>COUNTIF(Tabla1[ESTADO],"HACER")</f>
+        <f>COUNTIF(Planeacion[ESTADO],"HACER")</f>
         <v>0</v>
       </c>
       <c r="F11" s="17" t="s">
@@ -4403,7 +4456,7 @@
         <v>22</v>
       </c>
       <c r="D12" s="3">
-        <f>COUNTIF(Tabla1[ESTADO],"HACIENDO")</f>
+        <f>COUNTIF(Planeacion[ESTADO],"HACIENDO")</f>
         <v>0</v>
       </c>
       <c r="F12" s="21">
@@ -4421,7 +4474,7 @@
         <v>24</v>
       </c>
       <c r="D13" s="3">
-        <f>COUNTIF(Tabla1[ESTADO],"VERIFICAR")</f>
+        <f>COUNTIF(Planeacion[ESTADO],"VERIFICAR")</f>
         <v>0</v>
       </c>
       <c r="F13" s="21">
@@ -4439,7 +4492,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="3">
-        <f>COUNTIF(Tabla1[ESTADO],"HECHO")</f>
+        <f>COUNTIF(Planeacion[ESTADO],"HECHO")</f>
         <v>0</v>
       </c>
       <c r="F14" s="21">
@@ -4453,6 +4506,13 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C15" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="3">
+        <f>COUNTIF(Planeacion[ESTADO],"POSPUESTO")</f>
+        <v>0</v>
+      </c>
       <c r="F15" s="21">
         <v>4</v>
       </c>
@@ -4496,7 +4556,7 @@
   </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E7" xr:uid="{A3DCC8F9-4E73-E547-BE62-55E768E9A341}">
-      <formula1>"HACER, HACIENDO, HECHO, VERIFICAR"</formula1>
+      <formula1>"HACER, HACIENDO, HECHO, POSPUESTO, VERIFICAR"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D7" xr:uid="{865663F2-E980-3141-BCFB-41152B4A8D53}">
       <formula1>"ALEJANDRO GARCIA, BRANDON MEDINA, HELVER ROA , JOHAN MATOMA, PAULA VILLARREAL"</formula1>

</xml_diff>